<commit_message>
update specification table w/ exam info
</commit_message>
<xml_diff>
--- a/material/other/specification_tables_dprep.xlsx
+++ b/material/other/specification_tables_dprep.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tilburgu-my.sharepoint.com/personal/h_datta_tilburguniversity_edu/Documents/Teaching/dprep-08-fall/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannesdatta/research/course-dprep/material/other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="13_ncr:1_{25F7BD08-40A6-4FED-862B-2B24516424BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13E92740-340A-44A7-AF67-688613568FF9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BD90B7-2211-954A-961F-425052CA30EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="840" windowWidth="24460" windowHeight="16920" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exam (60%)" sheetId="1" r:id="rId1"/>
-    <sheet name="Team assignments (40%)" sheetId="2" r:id="rId2"/>
-    <sheet name="Explanation skills" sheetId="4" r:id="rId3"/>
+    <sheet name="new exam setup" sheetId="5" r:id="rId2"/>
+    <sheet name="Team assignments (40%)" sheetId="2" r:id="rId3"/>
+    <sheet name="Explanation skills" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Exam (60%)'!$A$1:$I$12</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Team assignments (40%)'!$A$1:$I$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Team assignments (40%)'!$A$1:$I$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -229,8 +230,226 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{84A234F8-A8AD-154C-B1BC-818C670DD521}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">S.Y.M. Koppelaar:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Some tips for the specification table:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">- Most important is to explain how the student has to prove a certain goal. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">- The verb in the learning goal refers to the highest cognitive skill (see sheet explanation skills).
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>- The points are the reward for the thinking process (the way). The lower cognitive skills are used to get to the highest cognitive skill.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{7EFADB51-6239-E443-A58D-50AC5386E0D4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">S. van Soest:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Students should be able to remember information and reproduce it. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{2CF10DA7-EC41-174A-9D6C-F21B895EE883}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">S. van Soest:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Students have to interpret the study material and give account of it in their own words. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{2B42A07A-560D-E046-8ABF-A7FA255A388B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">S. van Soest:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Students analyze and break up the study material and then relate the various pieces to each other. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{230F1D65-ED0B-4746-B324-8FE8C5BB9984}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">S. van Soest:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Students analyze and break up the study material and then relate the various pieces to each other. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{9B789D1D-0173-A34D-B191-DF152D26A418}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">S. van Soest:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Students give reasoned judgments of information on the basis of internal and external criteria, principles and ideas. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{3E663EB6-D5DD-C046-8506-422D80E9BC7C}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">S. van Soest:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Students bring components together to create something new/unique. (For example different theories, concepts, disciplines, models, or studies.)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
   <si>
     <t>Specification table</t>
   </si>
@@ -349,17 +568,80 @@
     <t>Computer exam (60%), open and closed questions</t>
   </si>
   <si>
-    <t>328059-M3 (fall, block 1; spring, block 3)</t>
-  </si>
-  <si>
     <t>Team assignment (40%; 8% individual component assessed via self- and peer assessment)</t>
+  </si>
+  <si>
+    <t>328059-M6 (fall, block 1; spring, block 3)</t>
+  </si>
+  <si>
+    <t>24m make fix</t>
+  </si>
+  <si>
+    <t>6m evaluation = 2MC</t>
+  </si>
+  <si>
+    <t>24m git commands</t>
+  </si>
+  <si>
+    <t>12m = 4 MC on evaluation</t>
+  </si>
+  <si>
+    <t>4 MC for evaluation based on book</t>
+  </si>
+  <si>
+    <t>closed/written</t>
+  </si>
+  <si>
+    <t>1q x 4 min / 4p</t>
+  </si>
+  <si>
+    <t>20m for doing dplyr</t>
+  </si>
+  <si>
+    <t>12P Rmarkdown plot + rendering APP</t>
+  </si>
+  <si>
+    <t>2 MC for comprehension x 3P</t>
+  </si>
+  <si>
+    <t>Tut/open</t>
+  </si>
+  <si>
+    <t>Closed/MC</t>
+  </si>
+  <si>
+    <t>N questions</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>2x 10</t>
+  </si>
+  <si>
+    <t>1x 24</t>
+  </si>
+  <si>
+    <t>1x 12</t>
+  </si>
+  <si>
+    <t>1x 4P</t>
+  </si>
+  <si>
+    <t>4x 3P</t>
+  </si>
+  <si>
+    <t>2x 3P</t>
+  </si>
+  <si>
+    <t>content tutorial question</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -424,6 +706,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -586,7 +874,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -667,22 +955,27 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1067,39 +1360,41 @@
   </sheetPr>
   <dimension ref="A1:AMJ19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="116" workbookViewId="0"/>
+    <sheetView zoomScale="114" zoomScaleNormal="85" zoomScaleSheetLayoutView="116" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:I12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="46.42578125" style="2" customWidth="1"/>
-    <col min="3" max="8" width="11.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="2" customWidth="1"/>
-    <col min="10" max="1024" width="20.140625" style="2"/>
+    <col min="1" max="1" width="2.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="46.5" style="2" customWidth="1"/>
+    <col min="3" max="8" width="11.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.5" style="2" customWidth="1"/>
+    <col min="10" max="1024" width="20.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -1108,7 +1403,7 @@
       <c r="I2" s="9"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="10" t="s">
@@ -1124,7 +1419,7 @@
       <c r="I3" s="11"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1024" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="4"/>
       <c r="C4" s="12" t="s">
@@ -1140,21 +1435,21 @@
       <c r="I4" s="14"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1024" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="15"/>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:1024" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1024" ht="77" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="17" t="s">
         <v>6</v>
@@ -1182,11 +1477,11 @@
       </c>
       <c r="J6" s="20"/>
     </row>
-    <row r="7" spans="1:1024" ht="57" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1024" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="16">
         <v>1</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="34" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="24"/>
@@ -1207,7 +1502,7 @@
       <c r="A8" s="16">
         <v>2</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="35" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="24"/>
@@ -1224,11 +1519,11 @@
       </c>
       <c r="J8" s="20"/>
     </row>
-    <row r="9" spans="1:1024" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1024" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="16">
         <v>3</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="34" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="24"/>
@@ -1247,11 +1542,11 @@
       </c>
       <c r="J9" s="20"/>
     </row>
-    <row r="10" spans="1:1024" ht="57" x14ac:dyDescent="0.25">
-      <c r="A10" s="37">
+    <row r="10" spans="1:1024" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="35">
         <v>4</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="34" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="24"/>
@@ -1270,7 +1565,7 @@
       </c>
       <c r="J10" s="20"/>
     </row>
-    <row r="11" spans="1:1024" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1024" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="16">
         <v>5</v>
       </c>
@@ -1293,7 +1588,7 @@
       </c>
       <c r="J11" s="20"/>
     </row>
-    <row r="12" spans="1:1024" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1024" ht="32" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="19" t="s">
         <v>14</v>
@@ -1328,37 +1623,37 @@
       </c>
       <c r="J12" s="20"/>
     </row>
-    <row r="14" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="AMG14"/>
       <c r="AMH14"/>
       <c r="AMI14"/>
       <c r="AMJ14"/>
     </row>
-    <row r="15" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="AMG15"/>
       <c r="AMH15"/>
       <c r="AMI15"/>
       <c r="AMJ15"/>
     </row>
-    <row r="16" spans="1:1024" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1024" x14ac:dyDescent="0.2">
       <c r="AMG16"/>
       <c r="AMH16"/>
       <c r="AMI16"/>
       <c r="AMJ16"/>
     </row>
-    <row r="17" spans="1021:1024" x14ac:dyDescent="0.25">
+    <row r="17" spans="1021:1024" x14ac:dyDescent="0.2">
       <c r="AMG17"/>
       <c r="AMH17"/>
       <c r="AMI17"/>
       <c r="AMJ17"/>
     </row>
-    <row r="18" spans="1021:1024" x14ac:dyDescent="0.25">
+    <row r="18" spans="1021:1024" x14ac:dyDescent="0.2">
       <c r="AMG18"/>
       <c r="AMH18"/>
       <c r="AMI18"/>
       <c r="AMJ18"/>
     </row>
-    <row r="19" spans="1021:1024" x14ac:dyDescent="0.25">
+    <row r="19" spans="1021:1024" x14ac:dyDescent="0.2">
       <c r="AMG19"/>
       <c r="AMH19"/>
       <c r="AMI19"/>
@@ -1376,40 +1671,342 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE3FF64-9A59-3F44-803A-E3E28FF0C262}">
+  <dimension ref="A1:R8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="50" customWidth="1"/>
+    <col min="3" max="9" width="11" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="O1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="106" x14ac:dyDescent="0.2">
+      <c r="A2" s="16"/>
+      <c r="B2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="45" x14ac:dyDescent="0.2">
+      <c r="A3" s="16">
+        <v>1</v>
+      </c>
+      <c r="B3" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24">
+        <v>0.2</v>
+      </c>
+      <c r="I3" s="23">
+        <v>0.2</v>
+      </c>
+      <c r="J3">
+        <f>120*I3</f>
+        <v>24</v>
+      </c>
+      <c r="L3" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="16">
+        <v>2</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="H4" s="24"/>
+      <c r="I4" s="23">
+        <v>0.1</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J7" si="0">120*I4</f>
+        <v>12</v>
+      </c>
+      <c r="M4" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="P4" t="s">
+        <v>59</v>
+      </c>
+      <c r="R4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="45" x14ac:dyDescent="0.2">
+      <c r="A5" s="16">
+        <v>3</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24">
+        <v>0.2</v>
+      </c>
+      <c r="G5" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="H5" s="24"/>
+      <c r="I5" s="23">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>36.000000000000007</v>
+      </c>
+      <c r="L5" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" t="s">
+        <v>56</v>
+      </c>
+      <c r="P5" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="45" x14ac:dyDescent="0.2">
+      <c r="A6" s="35">
+        <v>4</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="23">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>18.000000000000004</v>
+      </c>
+      <c r="L6" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" t="s">
+        <v>50</v>
+      </c>
+      <c r="O6" t="s">
+        <v>57</v>
+      </c>
+      <c r="P6" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="30" x14ac:dyDescent="0.2">
+      <c r="A7" s="16">
+        <v>5</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="36">
+        <v>0.2</v>
+      </c>
+      <c r="G7" s="24">
+        <v>0.05</v>
+      </c>
+      <c r="H7" s="24"/>
+      <c r="I7" s="23">
+        <v>0.25</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="L7" t="s">
+        <v>41</v>
+      </c>
+      <c r="M7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O7" t="s">
+        <v>56</v>
+      </c>
+      <c r="P7" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="31" x14ac:dyDescent="0.2">
+      <c r="A8" s="16"/>
+      <c r="B8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="33">
+        <v>0</v>
+      </c>
+      <c r="D8" s="33">
+        <v>0.05</v>
+      </c>
+      <c r="E8" s="33">
+        <v>0</v>
+      </c>
+      <c r="F8" s="33">
+        <v>0.5</v>
+      </c>
+      <c r="G8" s="33">
+        <v>0.25</v>
+      </c>
+      <c r="H8" s="33">
+        <v>0.2</v>
+      </c>
+      <c r="I8" s="21">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:I5"/>
+    <sheetView view="pageBreakPreview" zoomScale="107" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" style="2" customWidth="1"/>
-    <col min="3" max="8" width="11.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" style="2" customWidth="1"/>
-    <col min="10" max="1024" width="20.140625" style="2"/>
+    <col min="1" max="1" width="5.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="39.1640625" style="2" customWidth="1"/>
+    <col min="3" max="8" width="11.83203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.5" style="2" customWidth="1"/>
+    <col min="10" max="1024" width="20.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5"/>
       <c r="B1" s="4"/>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="4"/>
       <c r="C2" s="6" t="s">
@@ -1417,7 +2014,7 @@
       </c>
       <c r="D2" s="8" t="str">
         <f>'Exam (60%)'!D2</f>
-        <v>328059-M3 (fall, block 1; spring, block 3)</v>
+        <v>328059-M6 (fall, block 1; spring, block 3)</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -1426,7 +2023,7 @@
       <c r="I2" s="9"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="4"/>
       <c r="C3" s="10" t="s">
@@ -1443,14 +2040,14 @@
       <c r="I3" s="11"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="4"/>
       <c r="C4" s="12" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
@@ -1459,21 +2056,21 @@
       <c r="I4" s="14"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="15"/>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="76" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="17" t="s">
         <v>15</v>
@@ -1501,7 +2098,7 @@
       </c>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A7" s="19">
         <v>1</v>
       </c>
@@ -1522,7 +2119,7 @@
       </c>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" ht="57" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="19">
         <v>2</v>
       </c>
@@ -1543,7 +2140,7 @@
       </c>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="57" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A9" s="19">
         <v>3</v>
       </c>
@@ -1564,7 +2161,7 @@
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A10" s="19">
         <v>4</v>
       </c>
@@ -1585,7 +2182,7 @@
       </c>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="19">
         <v>5</v>
       </c>
@@ -1606,7 +2203,7 @@
       </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="31" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
       <c r="B12" s="19" t="s">
         <v>14</v>
@@ -1647,11 +2244,11 @@
     <mergeCell ref="C5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="94" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -1659,14 +2256,14 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="45.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="45.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
         <v>16</v>
       </c>
@@ -1677,7 +2274,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
         <v>7</v>
       </c>
@@ -1688,7 +2285,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
         <v>8</v>
       </c>
@@ -1699,7 +2296,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
         <v>10</v>
       </c>
@@ -1710,7 +2307,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>9</v>
       </c>
@@ -1721,7 +2318,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
         <v>11</v>
       </c>
@@ -1732,7 +2329,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
         <v>29</v>
       </c>

</xml_diff>